<commit_message>
Update Test_Case.xlsx with new test data and scenarios
</commit_message>
<xml_diff>
--- a/Test_Case.xlsx
+++ b/Test_Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ML_AI\Dự đoán giá nhà\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46419517-A61B-4922-9973-E6B245E63918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC03EBD-5EEE-411C-BD8C-902344310098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{D7E05346-DD7C-49D8-A336-C29990393CC2}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>